<commit_message>
added fresh report, delete and copy of report
</commit_message>
<xml_diff>
--- a/Data/Config_status.xlsx
+++ b/Data/Config_status.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -409,27 +409,64 @@
 QA Team</t>
   </si>
   <si>
-    <t>C:\Users\vamsikrishna.g\Documents\UiPath\Status\Data\Reportfor_status.xlsx</t>
-  </si>
-  <si>
-    <t>sowmya.jagadish@primefocus.com;vamsikrishna.g@primefocus.com;aditya.kulshreshtha@primefocus.com</t>
-  </si>
-  <si>
-    <t>Automation Report - For Status verification</t>
-  </si>
-  <si>
     <t>147871-119</t>
+  </si>
+  <si>
+    <t>Final_Reportpath</t>
+  </si>
+  <si>
+    <t>File_Rename</t>
+  </si>
+  <si>
+    <t>RenameFile</t>
+  </si>
+  <si>
+    <t>Automation Report - For AQC Status verification</t>
+  </si>
+  <si>
+    <t>C:\common\ReportforAQCStatus.xlsx</t>
+  </si>
+  <si>
+    <t>ReportforAQC-Status_</t>
+  </si>
+  <si>
+    <t>C:\common\Report\ReportforAQCStatus.xlsx</t>
+  </si>
+  <si>
+    <t>sowmya.jagadish@primefocus.com;vamsikrishna.g@primefocus.com</t>
+  </si>
+  <si>
+    <t>Backup_Report</t>
+  </si>
+  <si>
+    <t>C:\common\Backup</t>
+  </si>
+  <si>
+    <t>C:\common\Report\</t>
+  </si>
+  <si>
+    <t>RenameFile_B</t>
+  </si>
+  <si>
+    <t>C:\common\Backup\ReportforAQCStatus.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -458,18 +495,34 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,8 +541,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -549,32 +608,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -582,24 +653,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -884,25 +972,25 @@
   <dimension ref="A1:Z969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="12" customWidth="1"/>
     <col min="2" max="2" width="126.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="68.5703125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="18" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1"/>
@@ -930,362 +1018,384 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="22" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="26"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="26"/>
+    </row>
+    <row r="7" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="26"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="26"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="26"/>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="26"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="26"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="26"/>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="26"/>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="21"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="21"/>
-    </row>
-    <row r="7" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" s="21"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="21"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="21"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="21"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="21"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="21"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="21"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="14"/>
+      <c r="B14" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="22"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="22"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="17"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="13"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="13"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="13"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="21"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="21"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="21"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="14"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="21"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="14"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="21"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="14"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="21"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="21"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="21"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="21"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="21"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="21"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="21"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="14"/>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="21"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="21"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="21"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="14"/>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="21"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="14"/>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="21"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="21"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="21"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="14"/>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="21"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="14"/>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="21"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="14"/>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="21"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="14"/>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="21"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="14"/>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="21"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="14"/>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="21"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="14"/>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="21"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="14"/>
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="21"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="14"/>
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="21"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="14"/>
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="21"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="14"/>
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="21"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="14"/>
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="21"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="14"/>
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="21"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="14"/>
     </row>
     <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="21"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="14"/>
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="21"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="14"/>
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="21"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="14"/>
     </row>
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="21"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="14"/>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="21"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="14"/>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="21"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="14"/>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="12"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="21"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="14"/>
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="21"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="14"/>
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="21"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="14"/>
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="21"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="14"/>
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="21"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="14"/>
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3264,13 +3374,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="5"/>

</xml_diff>